<commit_message>
South Africa Data Update
</commit_message>
<xml_diff>
--- a/codeLibrary/R/R/airlineData/Cape Town.xlsx
+++ b/codeLibrary/R/R/airlineData/Cape Town.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Sites/LVM-Code/codeLibrary/R/R/airlineData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D97A4D37-C085-054C-9C2F-1069B0BBEAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897FD548-480F-F543-A279-CCB62B42E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37680" yWindow="5280" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="4720" yWindow="-19300" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>DateTime</t>
   </si>
@@ -133,16 +133,46 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>2021-11-30</t>
+  </si>
+  <si>
+    <t>2021-12-01</t>
+  </si>
+  <si>
+    <t>2021-12-02</t>
+  </si>
+  <si>
+    <t>2021-12-03</t>
+  </si>
+  <si>
+    <t>2021-12-04</t>
+  </si>
+  <si>
+    <t>2021-12-05</t>
+  </si>
+  <si>
+    <t>2021-12-06</t>
+  </si>
+  <si>
+    <t>2021-12-07</t>
+  </si>
+  <si>
+    <t>All flights departing after 12:01 a.m. ET December 6 will abide by a new CDC testing order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel bans announced on November 26 bar entry into the US of noncitizens coming from eight countries in southern Africa. They are Botswana, Eswatini, Lesotho, Malawi, Mozambique, Namibia, South Africa and Zimbabwe. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,6 +318,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +628,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -634,8 +672,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -646,9 +685,10 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -682,6 +722,7 @@
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
@@ -1002,14 +1043,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
@@ -1029,7 +1070,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1085,7 @@
         <v>0.73809523809523814</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1055,11 +1096,11 @@
         <v>68</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D31" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D39" si="0">C3/B3</f>
         <v>0.77272727272727271</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1074,7 +1115,7 @@
         <v>0.74358974358974361</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1130,7 @@
         <v>0.6987951807228916</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1104,7 +1145,7 @@
         <v>0.70329670329670335</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1119,7 +1160,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1134,7 +1175,7 @@
         <v>0.647887323943662</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1149,7 +1190,7 @@
         <v>0.64646464646464652</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1164,7 +1205,7 @@
         <v>0.62745098039215685</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1220,7 @@
         <v>0.6404494382022472</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1194,7 +1235,7 @@
         <v>0.62376237623762376</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1250,7 @@
         <v>0.63461538461538458</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1224,7 +1265,7 @@
         <v>0.6071428571428571</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1239,7 +1280,7 @@
         <v>0.620253164556962</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1254,7 +1295,7 @@
         <v>0.75824175824175821</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1269,7 +1310,7 @@
         <v>0.68085106382978722</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1284,7 +1325,7 @@
         <v>0.71264367816091956</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1299,7 +1340,7 @@
         <v>0.68085106382978722</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1314,7 +1355,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1370,7 @@
         <v>0.72115384615384615</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1344,7 +1385,7 @@
         <v>0.66216216216216217</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1359,7 +1400,7 @@
         <v>0.68085106382978722</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1415,7 @@
         <v>0.70652173913043481</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1430,7 @@
         <v>0.6741573033707865</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1404,7 +1445,7 @@
         <v>0.68421052631578949</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1460,7 @@
         <v>0.7010309278350515</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1433,8 +1474,11 @@
         <f t="shared" si="0"/>
         <v>0.71153846153846156</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1449,7 +1493,7 @@
         <v>0.69333333333333336</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1464,7 +1508,7 @@
         <v>0.68085106382978722</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1479,8 +1523,133 @@
         <v>0.65957446808510634</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2">
+        <v>86</v>
+      </c>
+      <c r="C32" s="2">
+        <v>56</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65116279069767447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2">
+        <v>103</v>
+      </c>
+      <c r="C33" s="2">
+        <v>60</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="0"/>
+        <v>0.58252427184466016</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2">
+        <v>64</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="0"/>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="2">
+        <v>114</v>
+      </c>
+      <c r="C35" s="2">
+        <v>71</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.6228070175438597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2">
+        <v>52</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.63414634146341464</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2">
+        <v>99</v>
+      </c>
+      <c r="C37" s="2">
+        <v>63</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2">
+        <v>99</v>
+      </c>
+      <c r="C38" s="2">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65656565656565657</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="2">
+        <v>90</v>
+      </c>
+      <c r="C39" s="2">
+        <v>56</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.62222222222222223</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F38" r:id="rId1" display="https://www.cdc.gov/coronavirus/2019-ncov/travelers/testing-international-air-travelers.html" xr:uid="{F63B89B2-D4CC-5440-B4B6-11A12295108C}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>